<commit_message>
fix empty tree items and remove ..
</commit_message>
<xml_diff>
--- a/Dialogue.xlsx
+++ b/Dialogue.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jams\dialogue-jam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{246A203F-F0C0-4E05-868F-144F9B002079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C068659-F46E-4AB2-9B23-0A1E325BC33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{31B0060E-BED8-46A8-967C-FDEF934619A9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{31B0060E-BED8-46A8-967C-FDEF934619A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Dialogue" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="110">
   <si>
     <t>Key</t>
   </si>
@@ -289,9 +302,6 @@
     <t>Verfication is easy after all. Please enter.</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
     <t>Alright so I don't know what's happening.</t>
   </si>
   <si>
@@ -301,9 +311,6 @@
     <t>So can you tell me?</t>
   </si>
   <si>
-    <t>...</t>
-  </si>
-  <si>
     <t>You don't know what's happening do you?</t>
   </si>
   <si>
@@ -316,7 +323,46 @@
     <t xml:space="preserve">It's clear you don't. </t>
   </si>
   <si>
-    <t>So…</t>
+    <t>I don't know what's happening.</t>
+  </si>
+  <si>
+    <t>Status?</t>
+  </si>
+  <si>
+    <t>Why?</t>
+  </si>
+  <si>
+    <t>[NO RESPONSE]</t>
+  </si>
+  <si>
+    <t>That's not what I meant.</t>
+  </si>
+  <si>
+    <t>How?</t>
+  </si>
+  <si>
+    <t>I don't see how that's relevant.</t>
+  </si>
+  <si>
+    <t>So what?</t>
+  </si>
+  <si>
+    <t>It seems that you are.</t>
+  </si>
+  <si>
+    <t>You souldn't be impaired.</t>
+  </si>
+  <si>
+    <t>Impairment is ill advised.</t>
+  </si>
+  <si>
+    <t>I'm not impaired.</t>
+  </si>
+  <si>
+    <t>Fine. There's music. So?</t>
+  </si>
+  <si>
+    <t>There is no music.</t>
   </si>
 </sst>
 </file>
@@ -847,7 +893,42 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1208,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EEF1E1D-7CD0-46E9-8BA9-075EA81969F2}">
   <dimension ref="A1:J212"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1887,13 +1968,19 @@
       <c r="B24" t="s">
         <v>50</v>
       </c>
+      <c r="C24" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" t="s">
+        <v>101</v>
+      </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>12211</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>12212</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="2"/>
@@ -1995,13 +2082,19 @@
       <c r="B28" t="s">
         <v>54</v>
       </c>
+      <c r="C28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" t="s">
+        <v>97</v>
+      </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>12221111</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>12221112</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="2"/>
@@ -3211,21 +3304,18 @@
         <v>13111</v>
       </c>
       <c r="B72" t="s">
+        <v>99</v>
+      </c>
+      <c r="C72" t="s">
         <v>89</v>
       </c>
-      <c r="C72" t="s">
-        <v>90</v>
-      </c>
-      <c r="D72" t="s">
-        <v>93</v>
-      </c>
       <c r="G72" t="str">
         <f t="shared" si="4"/>
         <v>131111</v>
       </c>
       <c r="H72" t="str">
         <f t="shared" si="5"/>
-        <v>131112</v>
+        <v/>
       </c>
       <c r="I72" t="str">
         <f t="shared" si="6"/>
@@ -3241,10 +3331,10 @@
         <v>131111</v>
       </c>
       <c r="B73" t="s">
+        <v>90</v>
+      </c>
+      <c r="C73" t="s">
         <v>91</v>
-      </c>
-      <c r="C73" t="s">
-        <v>92</v>
       </c>
       <c r="G73" t="str">
         <f t="shared" si="4"/>
@@ -3295,13 +3385,13 @@
         <v>131112</v>
       </c>
       <c r="B75" t="s">
+        <v>92</v>
+      </c>
+      <c r="C75" t="s">
+        <v>93</v>
+      </c>
+      <c r="D75" t="s">
         <v>94</v>
-      </c>
-      <c r="C75" t="s">
-        <v>95</v>
-      </c>
-      <c r="D75" t="s">
-        <v>96</v>
       </c>
       <c r="G75" t="str">
         <f t="shared" si="4"/>
@@ -3352,7 +3442,7 @@
         <v>1311122</v>
       </c>
       <c r="B77" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C77" t="s">
         <v>98</v>
@@ -3402,13 +3492,25 @@
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>12211</v>
+      </c>
+      <c r="B79" t="s">
+        <v>29</v>
+      </c>
+      <c r="C79" t="s">
+        <v>102</v>
+      </c>
+      <c r="D79" t="s">
+        <v>80</v>
+      </c>
       <c r="G79" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>122111</v>
       </c>
       <c r="H79" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>122112</v>
       </c>
       <c r="I79" t="str">
         <f t="shared" si="6"/>
@@ -3420,13 +3522,25 @@
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>12212</v>
+      </c>
+      <c r="B80" t="s">
+        <v>29</v>
+      </c>
+      <c r="C80" t="s">
+        <v>80</v>
+      </c>
+      <c r="D80" t="s">
+        <v>103</v>
+      </c>
       <c r="G80" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f>IF(C80&lt;&gt;$A80,IF(NOT(ISBLANK(C80)),_xlfn.CONCAT($A80,1),""),"")</f>
+        <v>122121</v>
       </c>
       <c r="H80" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>122122</v>
       </c>
       <c r="I80" t="str">
         <f t="shared" si="6"/>
@@ -3437,7 +3551,16 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>12221111</v>
+      </c>
+      <c r="B81" t="s">
+        <v>33</v>
+      </c>
+      <c r="C81">
+        <v>12221111</v>
+      </c>
       <c r="G81" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3455,7 +3578,16 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>12221112</v>
+      </c>
+      <c r="B82" t="s">
+        <v>33</v>
+      </c>
+      <c r="C82">
+        <v>12221112</v>
+      </c>
       <c r="G82" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3473,14 +3605,26 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>122111</v>
+      </c>
+      <c r="B83" t="s">
+        <v>104</v>
+      </c>
+      <c r="C83" t="s">
+        <v>108</v>
+      </c>
+      <c r="D83" t="s">
+        <v>109</v>
+      </c>
       <c r="G83" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1221111</v>
       </c>
       <c r="H83" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>1221112</v>
       </c>
       <c r="I83" t="str">
         <f t="shared" si="6"/>
@@ -3491,14 +3635,26 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>122112</v>
+      </c>
+      <c r="B84" t="s">
+        <v>105</v>
+      </c>
+      <c r="C84" t="s">
+        <v>107</v>
+      </c>
+      <c r="D84" t="s">
+        <v>43</v>
+      </c>
       <c r="G84" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1221121</v>
       </c>
       <c r="H84" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>1221122</v>
       </c>
       <c r="I84" t="str">
         <f t="shared" si="6"/>
@@ -3509,14 +3665,26 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>122121</v>
+      </c>
+      <c r="B85" t="s">
+        <v>106</v>
+      </c>
+      <c r="C85" t="s">
+        <v>107</v>
+      </c>
+      <c r="D85" t="s">
+        <v>43</v>
+      </c>
       <c r="G85" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1221211</v>
       </c>
       <c r="H85" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>1221212</v>
       </c>
       <c r="I85" t="str">
         <f t="shared" si="6"/>
@@ -3527,10 +3695,19 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>122122</v>
+      </c>
+      <c r="B86" t="s">
+        <v>104</v>
+      </c>
+      <c r="C86" t="s">
+        <v>109</v>
+      </c>
       <c r="G86" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1221221</v>
       </c>
       <c r="H86" t="str">
         <f t="shared" si="5"/>
@@ -3545,7 +3722,16 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>1221221</v>
+      </c>
+      <c r="B87" t="s">
+        <v>33</v>
+      </c>
+      <c r="C87">
+        <v>1221221</v>
+      </c>
       <c r="G87" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3563,7 +3749,16 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>1221121</v>
+      </c>
+      <c r="B88" t="s">
+        <v>33</v>
+      </c>
+      <c r="C88">
+        <v>1221121</v>
+      </c>
       <c r="G88" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3581,7 +3776,16 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>1221211</v>
+      </c>
+      <c r="B89" t="s">
+        <v>33</v>
+      </c>
+      <c r="C89">
+        <v>1221211</v>
+      </c>
       <c r="G89" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3599,7 +3803,16 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>1221111</v>
+      </c>
+      <c r="B90" t="s">
+        <v>33</v>
+      </c>
+      <c r="C90">
+        <v>1221111</v>
+      </c>
       <c r="G90" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3617,7 +3830,16 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>1221112</v>
+      </c>
+      <c r="B91" t="s">
+        <v>33</v>
+      </c>
+      <c r="C91">
+        <v>1221112</v>
+      </c>
       <c r="G91" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3635,7 +3857,16 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>1221122</v>
+      </c>
+      <c r="B92" t="s">
+        <v>33</v>
+      </c>
+      <c r="C92">
+        <v>1221122</v>
+      </c>
       <c r="G92" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3653,7 +3884,16 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>1221212</v>
+      </c>
+      <c r="B93" t="s">
+        <v>33</v>
+      </c>
+      <c r="C93">
+        <v>1221212</v>
+      </c>
       <c r="G93" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3671,7 +3911,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G94" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3689,7 +3929,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G95" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3707,7 +3947,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G96" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -5743,19 +5983,19 @@
     </row>
     <row r="209" spans="7:10" x14ac:dyDescent="0.35">
       <c r="G209" t="str">
-        <f t="shared" ref="G195:G212" si="16">IF(NOT(ISBLANK(C209)),_xlfn.CONCAT($A209,1),"")</f>
+        <f t="shared" ref="G209:G212" si="16">IF(NOT(ISBLANK(C209)),_xlfn.CONCAT($A209,1),"")</f>
         <v/>
       </c>
       <c r="H209" t="str">
-        <f t="shared" ref="H195:H212" si="17">IF(NOT(ISBLANK(D209)),_xlfn.CONCAT($A209,2),"")</f>
+        <f t="shared" ref="H209:H212" si="17">IF(NOT(ISBLANK(D209)),_xlfn.CONCAT($A209,2),"")</f>
         <v/>
       </c>
       <c r="I209" t="str">
-        <f t="shared" ref="I195:I212" si="18">IF(NOT(ISBLANK(E209)),_xlfn.CONCAT($A209,3),"")</f>
+        <f t="shared" ref="I209:I212" si="18">IF(NOT(ISBLANK(E209)),_xlfn.CONCAT($A209,3),"")</f>
         <v/>
       </c>
       <c r="J209" t="str">
-        <f t="shared" ref="J195:J212" si="19">IF(NOT(ISBLANK(F209)),_xlfn.CONCAT($A209,4),"")</f>
+        <f t="shared" ref="J209:J212" si="19">IF(NOT(ISBLANK(F209)),_xlfn.CONCAT($A209,4),"")</f>
         <v/>
       </c>
     </row>
@@ -5815,8 +6055,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:J208">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>COUNTIF($A:$A,G2) =0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C80 C83:C86 C94:C1048576">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>ISBLANK(C1)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>